<commit_message>
Update Stanleys Abenteuer Testergebnisse.xlsx
</commit_message>
<xml_diff>
--- a/Assets/Documents/Stanleys Abenteuer Testergebnisse.xlsx
+++ b/Assets/Documents/Stanleys Abenteuer Testergebnisse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\GitHub\HangedLarryStan\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55990AF7-351B-4AFB-A3D9-4BDB7D53F20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B412ED91-E7BC-4A5B-93DE-5522181F6924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>Stanleys Abenteuer Testergebnisse</t>
   </si>
@@ -87,13 +87,7 @@
     <t>??</t>
   </si>
   <si>
-    <t xml:space="preserve">Super, nur Tutorial vielleicht mit blinkenden Pfeilen; </t>
-  </si>
-  <si>
     <t>Grafik ist sehr unterschiedlich und der Wurm unscheinbar, aber ok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Super, nur Tutorial ist schlecht erkennbar; </t>
   </si>
   <si>
     <t>Super; Wurm unscheinbar, aber ok</t>
@@ -151,9 +145,6 @@
     <t>Super, Level 4 anpassen (Pfeile)</t>
   </si>
   <si>
-    <t>Super, Level 4 anpassen (Restpunkt prüfen)</t>
-  </si>
-  <si>
     <t>Tutorial: Gerade ausgehen in Level 2</t>
   </si>
   <si>
@@ -184,7 +175,22 @@
     <t>Folie Ausblicke: Animation mit laufenden Vogel</t>
   </si>
   <si>
-    <t>Wurde umgesetzt</t>
+    <t>Super, Level 4 anpassen (Resetpunkt prüfen)</t>
+  </si>
+  <si>
+    <t>Super, nur Tutorial ist schlecht erkennbar</t>
+  </si>
+  <si>
+    <t>Super, nur Tutorial vielleicht mit blinkenden Pfeilen</t>
+  </si>
+  <si>
+    <t>Erledigt</t>
+  </si>
+  <si>
+    <t>Weitere Animationen</t>
+  </si>
+  <si>
+    <t>In Arbeit</t>
   </si>
 </sst>
 </file>
@@ -272,6 +278,21 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -279,21 +300,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -578,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,15 +606,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
@@ -620,13 +626,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>2</v>
@@ -635,13 +641,13 @@
         <v>3</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="J5" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>8</v>
@@ -664,28 +670,28 @@
         <v>58</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -714,16 +720,16 @@
         <v>10</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -740,22 +746,22 @@
         <v>18</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>16</v>
@@ -765,63 +771,63 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="17">
         <v>4</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="15">
         <v>45678</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>52</v>
+      <c r="I9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="10">
         <v>45678</v>
@@ -830,7 +836,7 @@
         <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>5</v>
@@ -842,16 +848,16 @@
         <v>10</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -859,7 +865,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="10">
         <v>45678</v>
@@ -868,25 +874,25 @@
         <v>22</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>52</v>
@@ -897,7 +903,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C13" s="10">
         <v>45678</v>
@@ -906,7 +912,7 @@
         <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>5</v>
@@ -918,13 +924,13 @@
         <v>10</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>52</v>
@@ -947,11 +953,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="C9:C10"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
@@ -960,6 +961,11 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="C9:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>